<commit_message>
Adding missing values for GDP current and GDP growth
</commit_message>
<xml_diff>
--- a/WDIW_Dataset.xlsx
+++ b/WDIW_Dataset.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chase.kusterer/Desktop/Teaching/Python/Hult World Regions and Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/usuario/Documents/ES_Africa_T3/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7D80FC-F652-3448-839E-3FBD69357BEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="2260" windowWidth="28800" windowHeight="17540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
@@ -17,13 +18,10 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Raw!$A$1:$BO$218</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,6 +29,9 @@
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -1625,7 +1626,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1989,11 +1990,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:BO218"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B174" sqref="B174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2026,8 +2029,8 @@
     <col min="26" max="26" width="56.6640625" customWidth="1"/>
     <col min="27" max="27" width="56.5" customWidth="1"/>
     <col min="28" max="28" width="30.1640625" customWidth="1"/>
-    <col min="29" max="29" width="15" customWidth="1"/>
-    <col min="30" max="30" width="18.83203125" customWidth="1"/>
+    <col min="29" max="29" width="20" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="26.6640625" customWidth="1"/>
     <col min="32" max="32" width="59.6640625" customWidth="1"/>
     <col min="33" max="33" width="26.1640625" customWidth="1"/>
@@ -2268,7 +2271,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>65</v>
       </c>
@@ -2408,7 +2411,7 @@
         <v>3.4634074834735342</v>
       </c>
     </row>
-    <row r="3" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>66</v>
       </c>
@@ -2542,7 +2545,7 @@
         <v>1.541284963911691</v>
       </c>
     </row>
-    <row r="4" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>67</v>
       </c>
@@ -2676,7 +2679,7 @@
         <v>2.8713741406536588</v>
       </c>
     </row>
-    <row r="5" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>68</v>
       </c>
@@ -2726,7 +2729,7 @@
         <v>-0.24925596647667311</v>
       </c>
     </row>
-    <row r="6" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>69</v>
       </c>
@@ -2928,7 +2931,7 @@
         <v>4.3919572788704198</v>
       </c>
     </row>
-    <row r="8" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>71</v>
       </c>
@@ -3038,7 +3041,7 @@
         <v>0.41216145368397628</v>
       </c>
     </row>
-    <row r="9" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>72</v>
       </c>
@@ -3202,7 +3205,7 @@
         <v>1.1701959591143101</v>
       </c>
     </row>
-    <row r="10" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>73</v>
       </c>
@@ -3366,7 +3369,7 @@
         <v>0.32788567024530041</v>
       </c>
     </row>
-    <row r="11" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>74</v>
       </c>
@@ -3461,7 +3464,7 @@
         <v>0.70398038007724861</v>
       </c>
     </row>
-    <row r="12" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>75</v>
       </c>
@@ -3598,7 +3601,7 @@
         <v>1.8056636977842879</v>
       </c>
     </row>
-    <row r="13" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>76</v>
       </c>
@@ -3732,7 +3735,7 @@
         <v>1.0204786258452709</v>
       </c>
     </row>
-    <row r="14" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>77</v>
       </c>
@@ -3866,7 +3869,7 @@
         <v>1.5647733798107639</v>
       </c>
     </row>
-    <row r="15" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>78</v>
       </c>
@@ -3994,7 +3997,7 @@
         <v>1.120364692155067</v>
       </c>
     </row>
-    <row r="16" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>79</v>
       </c>
@@ -4125,7 +4128,7 @@
         <v>4.7857132162568874</v>
       </c>
     </row>
-    <row r="17" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>80</v>
       </c>
@@ -4265,7 +4268,7 @@
         <v>3.255244391899641</v>
       </c>
     </row>
-    <row r="18" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>81</v>
       </c>
@@ -4387,7 +4390,7 @@
         <v>4.3737909688750583E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>82</v>
       </c>
@@ -4548,7 +4551,7 @@
         <v>0.57279844402577684</v>
       </c>
     </row>
-    <row r="20" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>83</v>
       </c>
@@ -4682,7 +4685,7 @@
         <v>0.42811662435789699</v>
       </c>
     </row>
-    <row r="21" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>84</v>
       </c>
@@ -4953,7 +4956,7 @@
         <v>3.9092350513318892</v>
       </c>
     </row>
-    <row r="23" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>86</v>
       </c>
@@ -5015,7 +5018,7 @@
         <v>-1.0605180802662639</v>
       </c>
     </row>
-    <row r="24" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>87</v>
       </c>
@@ -5170,7 +5173,7 @@
         <v>3.0520623301063181</v>
       </c>
     </row>
-    <row r="25" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>88</v>
       </c>
@@ -5331,7 +5334,7 @@
         <v>1.9455435677378941</v>
       </c>
     </row>
-    <row r="26" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>89</v>
       </c>
@@ -5468,7 +5471,7 @@
         <v>-0.28061454849653839</v>
       </c>
     </row>
-    <row r="27" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>90</v>
       </c>
@@ -5602,7 +5605,7 @@
         <v>3.1930412549843621</v>
       </c>
     </row>
-    <row r="28" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>91</v>
       </c>
@@ -5766,7 +5769,7 @@
         <v>1.1169803463805099</v>
       </c>
     </row>
-    <row r="29" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>92</v>
       </c>
@@ -5819,7 +5822,7 @@
         <v>1.562025641015985</v>
       </c>
     </row>
-    <row r="30" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>93</v>
       </c>
@@ -5947,7 +5950,7 @@
         <v>1.5245016786041621</v>
       </c>
     </row>
-    <row r="31" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>94</v>
       </c>
@@ -6224,7 +6227,7 @@
         <v>5.0324024353619352</v>
       </c>
     </row>
-    <row r="33" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>96</v>
       </c>
@@ -6352,7 +6355,7 @@
         <v>5.7160124223008628</v>
       </c>
     </row>
-    <row r="34" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>98</v>
       </c>
@@ -6629,7 +6632,7 @@
         <v>3.7156097985851519</v>
       </c>
     </row>
-    <row r="36" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>100</v>
       </c>
@@ -6891,7 +6894,7 @@
         <v>1.9221342583633689</v>
       </c>
     </row>
-    <row r="38" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>101</v>
       </c>
@@ -7099,7 +7102,7 @@
         <v>2.1647560672223971</v>
       </c>
     </row>
-    <row r="40" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>103</v>
       </c>
@@ -7233,7 +7236,7 @@
         <v>3.8725295280713201</v>
       </c>
     </row>
-    <row r="41" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>104</v>
       </c>
@@ -7397,7 +7400,7 @@
         <v>1.502940612914837</v>
       </c>
     </row>
-    <row r="42" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>105</v>
       </c>
@@ -7531,7 +7534,7 @@
         <v>2.6935401382235411</v>
       </c>
     </row>
-    <row r="43" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>106</v>
       </c>
@@ -7951,7 +7954,7 @@
         <v>4.5729450882055156</v>
       </c>
     </row>
-    <row r="46" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>109</v>
       </c>
@@ -8085,7 +8088,7 @@
         <v>3.2621537322656349</v>
       </c>
     </row>
-    <row r="47" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>110</v>
       </c>
@@ -8386,7 +8389,7 @@
         <v>3.435977338931111</v>
       </c>
     </row>
-    <row r="49" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>112</v>
       </c>
@@ -8526,7 +8529,7 @@
         <v>-0.73363834777364689</v>
       </c>
     </row>
-    <row r="50" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>113</v>
       </c>
@@ -8660,7 +8663,7 @@
         <v>9.7680525306211213E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>114</v>
       </c>
@@ -8770,7 +8773,7 @@
         <v>0.24245323982721431</v>
       </c>
     </row>
-    <row r="52" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>115</v>
       </c>
@@ -8901,7 +8904,7 @@
         <v>0.74063851395412217</v>
       </c>
     </row>
-    <row r="53" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>116</v>
       </c>
@@ -9038,7 +9041,7 @@
         <v>0.40826543369626478</v>
       </c>
     </row>
-    <row r="54" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>117</v>
       </c>
@@ -9175,7 +9178,7 @@
         <v>0.77446118529360009</v>
       </c>
     </row>
-    <row r="55" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>118</v>
       </c>
@@ -9333,7 +9336,7 @@
         <v>1.754558927105252</v>
       </c>
     </row>
-    <row r="56" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>119</v>
       </c>
@@ -9407,7 +9410,7 @@
         <v>0.64213705479896677</v>
       </c>
     </row>
-    <row r="57" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>120</v>
       </c>
@@ -9544,7 +9547,7 @@
         <v>2.1567767127909212</v>
       </c>
     </row>
-    <row r="58" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>257</v>
       </c>
@@ -9675,7 +9678,7 @@
         <v>3.1526291544391509</v>
       </c>
     </row>
-    <row r="59" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>121</v>
       </c>
@@ -9836,7 +9839,7 @@
         <v>1.982365259206762</v>
       </c>
     </row>
-    <row r="60" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>122</v>
       </c>
@@ -9976,7 +9979,7 @@
         <v>2.0276289459987731</v>
       </c>
     </row>
-    <row r="61" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>123</v>
       </c>
@@ -10298,7 +10301,7 @@
         <v>4.4922620004669112</v>
       </c>
     </row>
-    <row r="63" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>125</v>
       </c>
@@ -10363,7 +10366,7 @@
         <v>117600</v>
       </c>
     </row>
-    <row r="64" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>126</v>
       </c>
@@ -10500,7 +10503,7 @@
         <v>0.3454666788774613</v>
       </c>
     </row>
-    <row r="65" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>127</v>
       </c>
@@ -10631,7 +10634,7 @@
         <v>1.667043631418093</v>
       </c>
     </row>
-    <row r="66" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>128</v>
       </c>
@@ -10768,7 +10771,7 @@
         <v>4.8738309519568084</v>
       </c>
     </row>
-    <row r="67" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>129</v>
       </c>
@@ -10842,7 +10845,7 @@
         <v>0.65375895270423479</v>
       </c>
     </row>
-    <row r="68" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>130</v>
       </c>
@@ -10973,7 +10976,7 @@
         <v>1.491917849482211</v>
       </c>
     </row>
-    <row r="69" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>131</v>
       </c>
@@ -11110,7 +11113,7 @@
         <v>0.29328796080298308</v>
       </c>
     </row>
-    <row r="70" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>132</v>
       </c>
@@ -11247,7 +11250,7 @@
         <v>0.33659025354372729</v>
       </c>
     </row>
-    <row r="71" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>133</v>
       </c>
@@ -11643,7 +11646,7 @@
         <v>4.0987451457513968</v>
       </c>
     </row>
-    <row r="74" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>136</v>
       </c>
@@ -11810,7 +11813,7 @@
         <v>0.69230371930422641</v>
       </c>
     </row>
-    <row r="75" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>137</v>
       </c>
@@ -12084,7 +12087,7 @@
         <v>3.4152108437049109</v>
       </c>
     </row>
-    <row r="77" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>139</v>
       </c>
@@ -12134,7 +12137,7 @@
         <v>-2.66805011587876E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>140</v>
       </c>
@@ -12268,7 +12271,7 @@
         <v>0.23121222602493899</v>
       </c>
     </row>
-    <row r="79" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>141</v>
       </c>
@@ -12342,7 +12345,7 @@
         <v>0.25944090654995888</v>
       </c>
     </row>
-    <row r="80" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>142</v>
       </c>
@@ -12452,7 +12455,7 @@
         <v>0.8088288595012153</v>
       </c>
     </row>
-    <row r="81" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>143</v>
       </c>
@@ -12559,7 +12562,7 @@
         <v>0.89943818809427212</v>
       </c>
     </row>
-    <row r="82" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>144</v>
       </c>
@@ -12967,7 +12970,7 @@
         <v>3.4960316373880089</v>
       </c>
     </row>
-    <row r="85" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>147</v>
       </c>
@@ -13101,7 +13104,7 @@
         <v>0.70975734597241968</v>
       </c>
     </row>
-    <row r="86" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>148</v>
       </c>
@@ -13226,7 +13229,7 @@
         <v>3.068597255474105</v>
       </c>
     </row>
-    <row r="87" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>149</v>
       </c>
@@ -13390,7 +13393,7 @@
         <v>2.8394746536215609</v>
       </c>
     </row>
-    <row r="88" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>150</v>
       </c>
@@ -13530,7 +13533,7 @@
         <v>0.74822290499903876</v>
       </c>
     </row>
-    <row r="89" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>151</v>
       </c>
@@ -13667,7 +13670,7 @@
         <v>0.1331771045643754</v>
       </c>
     </row>
-    <row r="90" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>152</v>
       </c>
@@ -13786,7 +13789,7 @@
         <v>2.385884023144345</v>
       </c>
     </row>
-    <row r="91" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>153</v>
       </c>
@@ -13920,7 +13923,7 @@
         <v>2.3144481259897769</v>
       </c>
     </row>
-    <row r="92" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>154</v>
       </c>
@@ -14084,7 +14087,7 @@
         <v>2.4084590939559969</v>
       </c>
     </row>
-    <row r="93" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>155</v>
       </c>
@@ -14221,7 +14224,7 @@
         <v>2.0786941392483529</v>
       </c>
     </row>
-    <row r="94" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>156</v>
       </c>
@@ -14352,7 +14355,7 @@
         <v>2.80303526619613</v>
       </c>
     </row>
-    <row r="95" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>157</v>
       </c>
@@ -14510,7 +14513,7 @@
         <v>1.422846879039249</v>
       </c>
     </row>
-    <row r="96" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>158</v>
       </c>
@@ -14560,7 +14563,7 @@
         <v>0.59234698465313906</v>
       </c>
     </row>
-    <row r="97" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>159</v>
       </c>
@@ -14697,7 +14700,7 @@
         <v>2.0254041595472669</v>
       </c>
     </row>
-    <row r="98" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>160</v>
       </c>
@@ -14834,7 +14837,7 @@
         <v>0.26299853978734539</v>
       </c>
     </row>
-    <row r="99" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>161</v>
       </c>
@@ -14974,7 +14977,7 @@
         <v>1.008524483831897</v>
       </c>
     </row>
-    <row r="100" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>162</v>
       </c>
@@ -15111,7 +15114,7 @@
         <v>-7.9234711822477585E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>163</v>
       </c>
@@ -15251,7 +15254,7 @@
         <v>2.621938695662422</v>
       </c>
     </row>
-    <row r="102" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>164</v>
       </c>
@@ -15415,7 +15418,7 @@
         <v>1.4860299602700771</v>
       </c>
     </row>
-    <row r="103" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>165</v>
       </c>
@@ -15555,7 +15558,7 @@
         <v>4.0922878595727772</v>
       </c>
     </row>
-    <row r="104" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>166</v>
       </c>
@@ -15671,7 +15674,7 @@
         <v>2.9779703897864538</v>
       </c>
     </row>
-    <row r="105" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>167</v>
       </c>
@@ -15781,7 +15784,7 @@
         <v>0.81803488916825595</v>
       </c>
     </row>
-    <row r="106" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>168</v>
       </c>
@@ -15915,7 +15918,7 @@
         <v>0.35698082709135459</v>
       </c>
     </row>
-    <row r="107" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>169</v>
       </c>
@@ -16010,7 +16013,7 @@
         <v>10887</v>
       </c>
     </row>
-    <row r="108" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>170</v>
       </c>
@@ -16147,7 +16150,7 @@
         <v>2.476711432354513</v>
       </c>
     </row>
-    <row r="109" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>171</v>
       </c>
@@ -16314,7 +16317,7 @@
         <v>2.4636636177689941</v>
       </c>
     </row>
-    <row r="110" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>172</v>
       </c>
@@ -16445,7 +16448,7 @@
         <v>3.4096393229929771</v>
       </c>
     </row>
-    <row r="111" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>173</v>
       </c>
@@ -16582,7 +16585,7 @@
         <v>-0.80690977693088062</v>
       </c>
     </row>
-    <row r="112" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>174</v>
       </c>
@@ -16719,7 +16722,7 @@
         <v>1.6746086953778381</v>
       </c>
     </row>
-    <row r="113" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>175</v>
       </c>
@@ -16993,7 +16996,7 @@
         <v>3.363342251293592</v>
       </c>
     </row>
-    <row r="115" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>177</v>
       </c>
@@ -17109,7 +17112,7 @@
         <v>1.702529016841652</v>
       </c>
     </row>
-    <row r="116" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>178</v>
       </c>
@@ -17174,7 +17177,7 @@
         <v>0.46309242711909387</v>
       </c>
     </row>
-    <row r="117" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>179</v>
       </c>
@@ -17308,7 +17311,7 @@
         <v>-1.175857291544846</v>
       </c>
     </row>
-    <row r="118" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>180</v>
       </c>
@@ -17442,7 +17445,7 @@
         <v>2.7257178634168628</v>
       </c>
     </row>
-    <row r="119" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>181</v>
       </c>
@@ -17564,7 +17567,7 @@
         <v>1.5782801764867911</v>
       </c>
     </row>
-    <row r="120" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>209</v>
       </c>
@@ -17704,7 +17707,7 @@
         <v>0.38099252352374391</v>
       </c>
     </row>
-    <row r="121" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>182</v>
       </c>
@@ -17838,7 +17841,7 @@
         <v>4.5202762883855279</v>
       </c>
     </row>
-    <row r="122" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>183</v>
       </c>
@@ -17978,7 +17981,7 @@
         <v>3.9188818294983769</v>
       </c>
     </row>
-    <row r="123" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>184</v>
       </c>
@@ -18118,7 +18121,7 @@
         <v>2.1679844803078372</v>
       </c>
     </row>
-    <row r="124" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>185</v>
       </c>
@@ -18243,7 +18246,7 @@
         <v>5.3869724309168792</v>
       </c>
     </row>
-    <row r="125" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>186</v>
       </c>
@@ -18380,7 +18383,7 @@
         <v>4.9152620720356657</v>
       </c>
     </row>
-    <row r="126" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>187</v>
       </c>
@@ -18511,7 +18514,7 @@
         <v>2.8084999901921579</v>
       </c>
     </row>
-    <row r="127" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>188</v>
       </c>
@@ -18585,7 +18588,7 @@
         <v>1.0892516906782861</v>
       </c>
     </row>
-    <row r="128" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>189</v>
       </c>
@@ -18853,7 +18856,7 @@
         <v>-7.8578013038997155E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>191</v>
       </c>
@@ -18990,7 +18993,7 @@
         <v>1.527731512523876</v>
       </c>
     </row>
-    <row r="131" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>192</v>
       </c>
@@ -19094,7 +19097,7 @@
         <v>1.4872540556552989</v>
       </c>
     </row>
-    <row r="132" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>193</v>
       </c>
@@ -19255,7 +19258,7 @@
         <v>3.045952184885747E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>194</v>
       </c>
@@ -19311,7 +19314,7 @@
         <v>0.84225341615383886</v>
       </c>
     </row>
-    <row r="134" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>195</v>
       </c>
@@ -19451,7 +19454,7 @@
         <v>1.957855034534618</v>
       </c>
     </row>
-    <row r="135" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>196</v>
       </c>
@@ -19582,7 +19585,7 @@
         <v>0.51809569540589073</v>
       </c>
     </row>
-    <row r="136" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>197</v>
       </c>
@@ -19719,7 +19722,7 @@
         <v>2.1761269787987079</v>
       </c>
     </row>
-    <row r="137" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>198</v>
       </c>
@@ -19856,7 +19859,7 @@
         <v>4.4038951118223917</v>
       </c>
     </row>
-    <row r="138" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>199</v>
       </c>
@@ -19996,7 +19999,7 @@
         <v>1.428613902958729</v>
       </c>
     </row>
-    <row r="139" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>210</v>
       </c>
@@ -20055,7 +20058,7 @@
         <v>0.75811552518140846</v>
       </c>
     </row>
-    <row r="140" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>200</v>
       </c>
@@ -20192,7 +20195,7 @@
         <v>4.0256074961249517</v>
       </c>
     </row>
-    <row r="141" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>201</v>
       </c>
@@ -20251,7 +20254,7 @@
         <v>-1.334638904354809</v>
       </c>
     </row>
-    <row r="142" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>202</v>
       </c>
@@ -20391,7 +20394,7 @@
         <v>3.392323442632037</v>
       </c>
     </row>
-    <row r="143" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>203</v>
       </c>
@@ -20528,7 +20531,7 @@
         <v>1.0776861057997089</v>
       </c>
     </row>
-    <row r="144" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>204</v>
       </c>
@@ -20629,7 +20632,7 @@
         <v>1.9859492384787789</v>
       </c>
     </row>
-    <row r="145" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>205</v>
       </c>
@@ -20757,7 +20760,7 @@
         <v>2.199327454334044</v>
       </c>
     </row>
-    <row r="146" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>206</v>
       </c>
@@ -20894,7 +20897,7 @@
         <v>1.634019876665461</v>
       </c>
     </row>
-    <row r="147" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>207</v>
       </c>
@@ -21168,7 +21171,7 @@
         <v>4.3103311784594966</v>
       </c>
     </row>
-    <row r="149" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>211</v>
       </c>
@@ -21305,7 +21308,7 @@
         <v>1.280246109298564</v>
       </c>
     </row>
-    <row r="150" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>212</v>
       </c>
@@ -21448,7 +21451,7 @@
         <v>5.3606024112884567</v>
       </c>
     </row>
-    <row r="151" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>213</v>
       </c>
@@ -21585,7 +21588,7 @@
         <v>2.6474018924498099</v>
       </c>
     </row>
-    <row r="152" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>214</v>
       </c>
@@ -21662,7 +21665,7 @@
         <v>1.210151442595609</v>
       </c>
     </row>
-    <row r="153" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>215</v>
       </c>
@@ -21817,7 +21820,7 @@
         <v>2.2145981377733812</v>
       </c>
     </row>
-    <row r="154" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>216</v>
       </c>
@@ -21942,7 +21945,7 @@
         <v>2.387830519345624</v>
       </c>
     </row>
-    <row r="155" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>217</v>
       </c>
@@ -22106,7 +22109,7 @@
         <v>1.755304885811076</v>
       </c>
     </row>
-    <row r="156" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>218</v>
       </c>
@@ -22279,7 +22282,7 @@
         <v>1.895094461229234</v>
       </c>
     </row>
-    <row r="157" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>219</v>
       </c>
@@ -22419,7 +22422,7 @@
         <v>1.8899045275895521</v>
       </c>
     </row>
-    <row r="158" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>220</v>
       </c>
@@ -22547,7 +22550,7 @@
         <v>-0.10890125804313509</v>
       </c>
     </row>
-    <row r="159" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>221</v>
       </c>
@@ -22684,7 +22687,7 @@
         <v>0.63542472129205374</v>
       </c>
     </row>
-    <row r="160" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>222</v>
       </c>
@@ -22833,7 +22836,7 @@
         <v>-2.4373952368848131</v>
       </c>
     </row>
-    <row r="161" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>223</v>
       </c>
@@ -22961,7 +22964,7 @@
         <v>2.679449988736144</v>
       </c>
     </row>
-    <row r="162" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>224</v>
       </c>
@@ -23101,7 +23104,7 @@
         <v>-0.51781942840419615</v>
       </c>
     </row>
-    <row r="163" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>225</v>
       </c>
@@ -23238,7 +23241,7 @@
         <v>0.27931318576073988</v>
       </c>
     </row>
-    <row r="164" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>226</v>
       </c>
@@ -23378,7 +23381,7 @@
         <v>3.043355690556373</v>
       </c>
     </row>
-    <row r="165" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>245</v>
       </c>
@@ -23452,7 +23455,7 @@
         <v>0.75836282100986396</v>
       </c>
     </row>
-    <row r="166" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>246</v>
       </c>
@@ -23574,7 +23577,7 @@
         <v>0.8049172959548474</v>
       </c>
     </row>
-    <row r="167" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>248</v>
       </c>
@@ -23702,7 +23705,7 @@
         <v>1.1334721944048201</v>
       </c>
     </row>
-    <row r="168" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>227</v>
       </c>
@@ -23824,7 +23827,7 @@
         <v>-0.81506799054279111</v>
       </c>
     </row>
-    <row r="169" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>228</v>
       </c>
@@ -24008,7 +24011,7 @@
         <v>3.1074060160514101</v>
       </c>
     </row>
-    <row r="171" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>230</v>
       </c>
@@ -24312,7 +24315,7 @@
         <v>3.755135273139901</v>
       </c>
     </row>
-    <row r="173" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>232</v>
       </c>
@@ -24696,7 +24699,7 @@
         <v>3.1389927390205878</v>
       </c>
     </row>
-    <row r="176" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>235</v>
       </c>
@@ -24827,7 +24830,7 @@
         <v>8.8595469992448453E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>236</v>
       </c>
@@ -24874,7 +24877,7 @@
         <v>1.502331373295319</v>
       </c>
     </row>
-    <row r="178" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>237</v>
       </c>
@@ -25011,7 +25014,7 @@
         <v>5.2927459313115488E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>238</v>
       </c>
@@ -25145,7 +25148,7 @@
         <v>0.53240430861274923</v>
       </c>
     </row>
-    <row r="180" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>239</v>
       </c>
@@ -25261,7 +25264,7 @@
         <v>4.6532876345678789</v>
       </c>
     </row>
-    <row r="181" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>240</v>
       </c>
@@ -25377,7 +25380,7 @@
         <v>4.1085453027759344</v>
       </c>
     </row>
-    <row r="182" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>241</v>
       </c>
@@ -25517,7 +25520,7 @@
         <v>2.1837113539144211</v>
       </c>
     </row>
-    <row r="183" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>242</v>
       </c>
@@ -25627,7 +25630,7 @@
         <v>2.0413550584760252</v>
       </c>
     </row>
-    <row r="184" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>243</v>
       </c>
@@ -25764,7 +25767,7 @@
         <v>0.53579908474322591</v>
       </c>
     </row>
-    <row r="185" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>244</v>
       </c>
@@ -25910,7 +25913,7 @@
         <v>1.5281048955345109</v>
       </c>
     </row>
-    <row r="186" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>247</v>
       </c>
@@ -25963,7 +25966,7 @@
         <v>54.4</v>
       </c>
     </row>
-    <row r="187" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>249</v>
       </c>
@@ -26091,7 +26094,7 @@
         <v>3.1223244476912</v>
       </c>
     </row>
-    <row r="188" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>250</v>
       </c>
@@ -26219,7 +26222,7 @@
         <v>0.98932140458844431</v>
       </c>
     </row>
-    <row r="189" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>251</v>
       </c>
@@ -26353,7 +26356,7 @@
         <v>1.6853721019236789</v>
       </c>
     </row>
-    <row r="190" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>252</v>
       </c>
@@ -26487,7 +26490,7 @@
         <v>0.96298643902389491</v>
       </c>
     </row>
-    <row r="191" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>253</v>
       </c>
@@ -26597,7 +26600,7 @@
         <v>-0.98517853847325876</v>
       </c>
     </row>
-    <row r="192" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>254</v>
       </c>
@@ -26749,7 +26752,7 @@
         <v>2.9570596604595991</v>
       </c>
     </row>
-    <row r="193" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>255</v>
       </c>
@@ -26886,7 +26889,7 @@
         <v>5.1977838804640424</v>
       </c>
     </row>
-    <row r="194" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>256</v>
       </c>
@@ -27044,7 +27047,7 @@
         <v>1.88549585655688</v>
       </c>
     </row>
-    <row r="195" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>258</v>
       </c>
@@ -27181,7 +27184,7 @@
         <v>3.7851209241531811</v>
       </c>
     </row>
-    <row r="196" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>259</v>
       </c>
@@ -27294,7 +27297,7 @@
         <v>0.62398063100654688</v>
       </c>
     </row>
-    <row r="197" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>260</v>
       </c>
@@ -27425,7 +27428,7 @@
         <v>0.38681662355831131</v>
       </c>
     </row>
-    <row r="198" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>261</v>
       </c>
@@ -27559,7 +27562,7 @@
         <v>1.5712340608553319</v>
       </c>
     </row>
-    <row r="199" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>262</v>
       </c>
@@ -27696,7 +27699,7 @@
         <v>2.2766464722812709</v>
       </c>
     </row>
-    <row r="200" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>263</v>
       </c>
@@ -27815,7 +27818,7 @@
         <v>2.503281482210971</v>
       </c>
     </row>
-    <row r="201" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>264</v>
       </c>
@@ -27880,7 +27883,7 @@
         <v>1.8338925017437211</v>
       </c>
     </row>
-    <row r="202" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>265</v>
       </c>
@@ -27939,7 +27942,7 @@
         <v>2.7387062690541319</v>
       </c>
     </row>
-    <row r="203" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>266</v>
       </c>
@@ -28079,7 +28082,7 @@
         <v>6.2467245002382823</v>
       </c>
     </row>
-    <row r="204" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>267</v>
       </c>
@@ -28219,7 +28222,7 @@
         <v>-0.25333361466552717</v>
       </c>
     </row>
-    <row r="205" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>268</v>
       </c>
@@ -28350,7 +28353,7 @@
         <v>1.668055850912834</v>
       </c>
     </row>
-    <row r="206" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>269</v>
       </c>
@@ -28487,7 +28490,7 @@
         <v>1.0133905443011371</v>
       </c>
     </row>
-    <row r="207" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>270</v>
       </c>
@@ -28621,7 +28624,7 @@
         <v>0.87960012267458643</v>
       </c>
     </row>
-    <row r="208" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
         <v>271</v>
       </c>
@@ -28812,7 +28815,7 @@
         <v>0.46566278974760678</v>
       </c>
     </row>
-    <row r="209" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
         <v>272</v>
       </c>
@@ -28949,7 +28952,7 @@
         <v>1.4858781399267851</v>
       </c>
     </row>
-    <row r="210" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
         <v>273</v>
       </c>
@@ -29068,7 +29071,7 @@
         <v>2.9494079867449461</v>
       </c>
     </row>
-    <row r="211" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>274</v>
       </c>
@@ -29181,7 +29184,7 @@
         <v>-1.5184311536214641</v>
       </c>
     </row>
-    <row r="212" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>275</v>
       </c>
@@ -29315,7 +29318,7 @@
         <v>3.0344161048120779</v>
       </c>
     </row>
-    <row r="213" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>276</v>
       </c>
@@ -29419,7 +29422,7 @@
         <v>-9.746494470441816E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>277</v>
       </c>
@@ -29532,7 +29535,7 @@
         <v>2.339808980695099</v>
       </c>
     </row>
-    <row r="215" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
         <v>278</v>
       </c>
@@ -29672,7 +29675,7 @@
         <v>1.9851354584988601</v>
       </c>
     </row>
-    <row r="216" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>279</v>
       </c>
@@ -29803,7 +29806,7 @@
         <v>4.1661233621407341</v>
       </c>
     </row>
-    <row r="217" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
         <v>280</v>
       </c>
@@ -29940,7 +29943,7 @@
         <v>4.2113486531420703</v>
       </c>
     </row>
-    <row r="218" spans="1:67" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:67" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
         <v>281</v>
       </c>
@@ -30081,7 +30084,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BO218"/>
+  <autoFilter ref="A1:BO218" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Sideswipe"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>